<commit_message>
Bunch of edits to figures
</commit_message>
<xml_diff>
--- a/data/YBFMP_WQ_Data_WORKING_20221006.xlsx
+++ b/data/YBFMP_WQ_Data_WORKING_20221006.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\YOLO BYPASS DATA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3D99EF2-AE56-4203-B52E-0DD53F81AD01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA12FAF7-6D08-4C10-B459-44950204AC47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="478" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14445" yWindow="-16200" windowWidth="14400" windowHeight="15600" tabRatio="478" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="3" r:id="rId1"/>
@@ -202,7 +202,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5225" uniqueCount="992">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5420" uniqueCount="1018">
   <si>
     <t>Run Name</t>
   </si>
@@ -3415,18 +3415,12 @@
     <t>ES0923B0565</t>
   </si>
   <si>
-    <t>PH,GS,JS,PD</t>
-  </si>
-  <si>
     <t>ES0923B0566</t>
   </si>
   <si>
     <t>ES0923B0567</t>
   </si>
   <si>
-    <t>FALASE</t>
-  </si>
-  <si>
     <t>ES0923B0568</t>
   </si>
   <si>
@@ -3437,6 +3431,90 @@
   </si>
   <si>
     <t>last measurement taken @ total depth of pole.</t>
+  </si>
+  <si>
+    <t>ES0923B0578</t>
+  </si>
+  <si>
+    <t>lwigger, lolson</t>
+  </si>
+  <si>
+    <t>ES0923B0584</t>
+  </si>
+  <si>
+    <t>aevans, lvance</t>
+  </si>
+  <si>
+    <t>ES0923B0579</t>
+  </si>
+  <si>
+    <t>lolson, lwigger</t>
+  </si>
+  <si>
+    <t>Lots of veg (ludwigia)</t>
+  </si>
+  <si>
+    <t>ES0923B0580</t>
+  </si>
+  <si>
+    <t>lolson, molinger</t>
+  </si>
+  <si>
+    <t>ES0923B0581</t>
+  </si>
+  <si>
+    <t>ES0923B0582</t>
+  </si>
+  <si>
+    <t>lvance, aevans</t>
+  </si>
+  <si>
+    <t>ES0923B0583</t>
+  </si>
+  <si>
+    <t>jcasby, aevans</t>
+  </si>
+  <si>
+    <t>ES0923B0585</t>
+  </si>
+  <si>
+    <t>EL,AH,GS,JS</t>
+  </si>
+  <si>
+    <t>ES0923B0586</t>
+  </si>
+  <si>
+    <t>GS</t>
+  </si>
+  <si>
+    <t>AH,GS,JS</t>
+  </si>
+  <si>
+    <t>ES0923B0587</t>
+  </si>
+  <si>
+    <t>ES0923B0588</t>
+  </si>
+  <si>
+    <t>ES0923B0589</t>
+  </si>
+  <si>
+    <t>ES0923B0590</t>
+  </si>
+  <si>
+    <t>Final measurement taken @full length of pole (2.19 m)</t>
+  </si>
+  <si>
+    <t>Corrected avg. turb from 43.5 to 42.5</t>
+  </si>
+  <si>
+    <t>PH,GS,JS,DD</t>
+  </si>
+  <si>
+    <t>Changed initials PD to DD</t>
+  </si>
+  <si>
+    <t>date changed from 9/6 to 9/7</t>
   </si>
 </sst>
 </file>
@@ -4125,10 +4203,10 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:AX393"/>
+  <dimension ref="A1:AX406"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AV1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A386" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="AT1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A376" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
       <selection pane="bottomLeft" activeCell="AX393" sqref="AX393"/>
     </sheetView>
@@ -46339,7 +46417,7 @@
         <v>1</v>
       </c>
       <c r="AC383" s="1">
-        <v>43.5</v>
+        <v>42.5</v>
       </c>
       <c r="AM383" s="1" t="s">
         <v>740</v>
@@ -46365,8 +46443,14 @@
       <c r="AT383" s="1" t="b">
         <v>1</v>
       </c>
+      <c r="AV383" s="1" t="s">
+        <v>1014</v>
+      </c>
       <c r="AW383" s="1" t="s">
         <v>582</v>
+      </c>
+      <c r="AX383" s="1" t="s">
+        <v>987</v>
       </c>
     </row>
     <row r="384" spans="3:50" x14ac:dyDescent="0.35">
@@ -46466,8 +46550,11 @@
       <c r="AW384" s="1" t="s">
         <v>582</v>
       </c>
+      <c r="AX384" s="1" t="s">
+        <v>987</v>
+      </c>
     </row>
-    <row r="385" spans="3:49" x14ac:dyDescent="0.35">
+    <row r="385" spans="3:50" x14ac:dyDescent="0.35">
       <c r="C385" s="1" t="s">
         <v>255</v>
       </c>
@@ -46564,8 +46651,11 @@
       <c r="AW385" s="1" t="s">
         <v>582</v>
       </c>
+      <c r="AX385" s="1" t="s">
+        <v>987</v>
+      </c>
     </row>
-    <row r="386" spans="3:49" x14ac:dyDescent="0.35">
+    <row r="386" spans="3:50" x14ac:dyDescent="0.35">
       <c r="C386" s="1" t="s">
         <v>255</v>
       </c>
@@ -46659,8 +46749,11 @@
       <c r="AW386" s="1" t="s">
         <v>582</v>
       </c>
+      <c r="AX386" s="1" t="s">
+        <v>987</v>
+      </c>
     </row>
-    <row r="387" spans="3:49" x14ac:dyDescent="0.35">
+    <row r="387" spans="3:50" x14ac:dyDescent="0.35">
       <c r="C387" s="1" t="s">
         <v>255</v>
       </c>
@@ -46760,8 +46853,11 @@
       <c r="AW387" s="1" t="s">
         <v>582</v>
       </c>
+      <c r="AX387" s="1" t="s">
+        <v>987</v>
+      </c>
     </row>
-    <row r="388" spans="3:49" x14ac:dyDescent="0.35">
+    <row r="388" spans="3:50" x14ac:dyDescent="0.35">
       <c r="C388" s="1" t="s">
         <v>383</v>
       </c>
@@ -46855,8 +46951,11 @@
       <c r="AW388" s="1" t="s">
         <v>582</v>
       </c>
+      <c r="AX388" s="1" t="s">
+        <v>987</v>
+      </c>
     </row>
-    <row r="389" spans="3:49" x14ac:dyDescent="0.35">
+    <row r="389" spans="3:50" x14ac:dyDescent="0.35">
       <c r="C389" s="1" t="s">
         <v>383</v>
       </c>
@@ -46983,8 +47082,11 @@
       <c r="AW389" s="1" t="s">
         <v>582</v>
       </c>
+      <c r="AX389" s="1" t="s">
+        <v>987</v>
+      </c>
     </row>
-    <row r="390" spans="3:49" x14ac:dyDescent="0.35">
+    <row r="390" spans="3:50" x14ac:dyDescent="0.35">
       <c r="C390" s="1" t="s">
         <v>982</v>
       </c>
@@ -47013,7 +47115,7 @@
         <v>603</v>
       </c>
       <c r="P390" s="1" t="s">
-        <v>984</v>
+        <v>1015</v>
       </c>
       <c r="Q390" s="3">
         <v>3</v>
@@ -47078,11 +47180,17 @@
       <c r="AT390" s="1" t="b">
         <v>1</v>
       </c>
+      <c r="AV390" s="1" t="s">
+        <v>1016</v>
+      </c>
       <c r="AW390" s="1" t="s">
         <v>582</v>
       </c>
+      <c r="AX390" s="1" t="s">
+        <v>987</v>
+      </c>
     </row>
-    <row r="391" spans="3:49" x14ac:dyDescent="0.35">
+    <row r="391" spans="3:50" x14ac:dyDescent="0.35">
       <c r="C391" s="1" t="s">
         <v>255</v>
       </c>
@@ -47090,7 +47198,7 @@
         <v>14</v>
       </c>
       <c r="F391" s="1" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="G391" s="2">
         <v>45175</v>
@@ -47111,7 +47219,7 @@
         <v>603</v>
       </c>
       <c r="P391" s="1" t="s">
-        <v>984</v>
+        <v>1015</v>
       </c>
       <c r="Q391" s="3">
         <v>3</v>
@@ -47135,7 +47243,7 @@
         <v>140</v>
       </c>
       <c r="X391" s="1">
-        <v>9.5</v>
+        <v>7.5</v>
       </c>
       <c r="Y391" s="1" t="s">
         <v>73</v>
@@ -47176,11 +47284,17 @@
       <c r="AT391" s="1" t="b">
         <v>1</v>
       </c>
+      <c r="AV391" s="1" t="s">
+        <v>1016</v>
+      </c>
       <c r="AW391" s="1" t="s">
         <v>582</v>
       </c>
+      <c r="AX391" s="1" t="s">
+        <v>987</v>
+      </c>
     </row>
-    <row r="392" spans="3:49" x14ac:dyDescent="0.35">
+    <row r="392" spans="3:50" x14ac:dyDescent="0.35">
       <c r="C392" s="1" t="s">
         <v>255</v>
       </c>
@@ -47188,7 +47302,7 @@
         <v>97</v>
       </c>
       <c r="F392" s="1" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="G392" s="2">
         <v>45175</v>
@@ -47209,7 +47323,7 @@
         <v>603</v>
       </c>
       <c r="P392" s="1" t="s">
-        <v>984</v>
+        <v>1015</v>
       </c>
       <c r="Q392" s="3">
         <v>3</v>
@@ -47254,7 +47368,7 @@
         <v>740</v>
       </c>
       <c r="AN392" s="1" t="s">
-        <v>987</v>
+        <v>740</v>
       </c>
       <c r="AO392" s="1" t="b">
         <v>0</v>
@@ -47273,12 +47387,18 @@
       </c>
       <c r="AT392" s="1" t="b">
         <v>1</v>
+      </c>
+      <c r="AV392" s="1" t="s">
+        <v>1016</v>
       </c>
       <c r="AW392" s="1" t="s">
         <v>582</v>
       </c>
+      <c r="AX392" s="1" t="s">
+        <v>987</v>
+      </c>
     </row>
-    <row r="393" spans="3:49" x14ac:dyDescent="0.35">
+    <row r="393" spans="3:50" x14ac:dyDescent="0.35">
       <c r="C393" s="1" t="s">
         <v>383</v>
       </c>
@@ -47286,10 +47406,10 @@
         <v>13</v>
       </c>
       <c r="F393" s="1" t="s">
-        <v>988</v>
+        <v>986</v>
       </c>
       <c r="G393" s="2">
-        <v>45175</v>
+        <v>45176</v>
       </c>
       <c r="H393" s="50">
         <v>0.38472222222222219</v>
@@ -47298,7 +47418,7 @@
         <v>7</v>
       </c>
       <c r="M393" s="1" t="s">
-        <v>989</v>
+        <v>987</v>
       </c>
       <c r="N393" s="1" t="s">
         <v>225</v>
@@ -47307,7 +47427,7 @@
         <v>571</v>
       </c>
       <c r="P393" s="1" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
       <c r="Q393" s="3">
         <v>1</v>
@@ -47351,6 +47471,30 @@
       <c r="AD393" s="1">
         <v>1815.9</v>
       </c>
+      <c r="AE393" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="AF393" s="1">
+        <v>0.26</v>
+      </c>
+      <c r="AG393" s="1">
+        <v>0.72</v>
+      </c>
+      <c r="AH393" s="1">
+        <v>2.19</v>
+      </c>
+      <c r="AI393" s="1">
+        <v>1368</v>
+      </c>
+      <c r="AJ393" s="1">
+        <v>909.4</v>
+      </c>
+      <c r="AK393" s="1">
+        <v>453.9</v>
+      </c>
+      <c r="AL393" s="1">
+        <v>49.85</v>
+      </c>
       <c r="AM393" s="1" t="b">
         <v>1</v>
       </c>
@@ -47376,7 +47520,1353 @@
         <v>1</v>
       </c>
       <c r="AU393" s="1" t="s">
+        <v>989</v>
+      </c>
+      <c r="AV393" s="1" t="s">
+        <v>1017</v>
+      </c>
+      <c r="AW393" s="1" t="s">
+        <v>582</v>
+      </c>
+      <c r="AX393" s="1" t="s">
+        <v>987</v>
+      </c>
+    </row>
+    <row r="394" spans="3:50" x14ac:dyDescent="0.35">
+      <c r="C394" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="D394" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F394" s="1" t="s">
+        <v>990</v>
+      </c>
+      <c r="G394" s="2">
+        <v>45188</v>
+      </c>
+      <c r="H394" s="50">
+        <v>0.4465277777777778</v>
+      </c>
+      <c r="L394" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M394" s="1" t="s">
+        <v>693</v>
+      </c>
+      <c r="N394" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="O394" s="1" t="s">
+        <v>582</v>
+      </c>
+      <c r="P394" s="1" t="s">
         <v>991</v>
+      </c>
+      <c r="Q394" s="3">
+        <v>1</v>
+      </c>
+      <c r="R394" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="S394" s="1">
+        <v>0.23</v>
+      </c>
+      <c r="T394" s="4">
+        <v>23</v>
+      </c>
+      <c r="U394" s="1">
+        <v>6.43</v>
+      </c>
+      <c r="V394" s="1">
+        <v>588</v>
+      </c>
+      <c r="W394" s="1">
+        <v>565</v>
+      </c>
+      <c r="X394" s="1">
+        <v>7.77</v>
+      </c>
+      <c r="Y394" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="Z394" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="AA394" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB394" s="1">
+        <v>2</v>
+      </c>
+      <c r="AC394" s="1">
+        <v>34.200000000000003</v>
+      </c>
+      <c r="AM394" s="1" t="s">
+        <v>740</v>
+      </c>
+      <c r="AN394" s="1" t="s">
+        <v>740</v>
+      </c>
+      <c r="AO394" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP394" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AQ394" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AR394" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AS394" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AT394" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AW394" s="1" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="395" spans="3:50" x14ac:dyDescent="0.35">
+      <c r="C395" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="D395" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F395" s="1" t="s">
+        <v>994</v>
+      </c>
+      <c r="G395" s="2">
+        <v>45188</v>
+      </c>
+      <c r="H395" s="50">
+        <v>0.3923611111111111</v>
+      </c>
+      <c r="L395" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M395" s="1" t="s">
+        <v>693</v>
+      </c>
+      <c r="N395" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="O395" s="1" t="s">
+        <v>582</v>
+      </c>
+      <c r="P395" s="1" t="s">
+        <v>995</v>
+      </c>
+      <c r="Q395" s="3">
+        <v>1</v>
+      </c>
+      <c r="R395" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="S395" s="1">
+        <v>0.22</v>
+      </c>
+      <c r="T395" s="4">
+        <v>21.9</v>
+      </c>
+      <c r="U395" s="1">
+        <v>4.34</v>
+      </c>
+      <c r="V395" s="1">
+        <v>837</v>
+      </c>
+      <c r="W395" s="1">
+        <v>788</v>
+      </c>
+      <c r="X395" s="1">
+        <v>7.37</v>
+      </c>
+      <c r="Y395" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="Z395" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="AA395" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB395" s="1">
+        <v>3</v>
+      </c>
+      <c r="AC395" s="1">
+        <v>34.200000000000003</v>
+      </c>
+      <c r="AM395" s="1" t="s">
+        <v>740</v>
+      </c>
+      <c r="AN395" s="1" t="s">
+        <v>740</v>
+      </c>
+      <c r="AO395" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP395" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AQ395" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AR395" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AS395" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AT395" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AU395" s="1" t="s">
+        <v>996</v>
+      </c>
+      <c r="AW395" s="1" t="s">
+        <v>987</v>
+      </c>
+      <c r="AX395" s="1" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="396" spans="3:50" x14ac:dyDescent="0.35">
+      <c r="C396" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="D396" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F396" s="1" t="s">
+        <v>997</v>
+      </c>
+      <c r="G396" s="2">
+        <v>45188</v>
+      </c>
+      <c r="H396" s="50">
+        <v>0.31805555555555554</v>
+      </c>
+      <c r="L396" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M396" s="1" t="s">
+        <v>843</v>
+      </c>
+      <c r="N396" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="O396" s="1" t="s">
+        <v>582</v>
+      </c>
+      <c r="P396" s="1" t="s">
+        <v>998</v>
+      </c>
+      <c r="Q396" s="3">
+        <v>1</v>
+      </c>
+      <c r="R396" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="S396" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="T396" s="4">
+        <v>21.4</v>
+      </c>
+      <c r="U396" s="1">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="V396" s="1">
+        <v>631</v>
+      </c>
+      <c r="W396" s="1">
+        <v>587</v>
+      </c>
+      <c r="X396" s="1">
+        <v>7.27</v>
+      </c>
+      <c r="Y396" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="Z396" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="AA396" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB396" s="1">
+        <v>2</v>
+      </c>
+      <c r="AC396" s="1">
+        <v>20.8</v>
+      </c>
+      <c r="AM396" s="1" t="s">
+        <v>740</v>
+      </c>
+      <c r="AN396" s="1" t="s">
+        <v>740</v>
+      </c>
+      <c r="AO396" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP396" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AQ396" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AR396" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AS396" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AT396" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AW396" s="1" t="s">
+        <v>987</v>
+      </c>
+      <c r="AX396" s="1" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="397" spans="3:50" x14ac:dyDescent="0.35">
+      <c r="C397" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="D397" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F397" s="1" t="s">
+        <v>999</v>
+      </c>
+      <c r="G397" s="2">
+        <v>45188</v>
+      </c>
+      <c r="H397" s="50">
+        <v>0.54236111111111118</v>
+      </c>
+      <c r="L397" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M397" s="1" t="s">
+        <v>693</v>
+      </c>
+      <c r="N397" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="O397" s="1" t="s">
+        <v>582</v>
+      </c>
+      <c r="P397" s="1" t="s">
+        <v>995</v>
+      </c>
+      <c r="Q397" s="3">
+        <v>1</v>
+      </c>
+      <c r="R397" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="S397" s="1">
+        <v>0.18</v>
+      </c>
+      <c r="T397" s="4">
+        <v>21.4</v>
+      </c>
+      <c r="U397" s="1">
+        <v>4.8499999999999996</v>
+      </c>
+      <c r="V397" s="1">
+        <v>519</v>
+      </c>
+      <c r="W397" s="1">
+        <v>483</v>
+      </c>
+      <c r="X397" s="1">
+        <v>7.62</v>
+      </c>
+      <c r="Y397" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="Z397" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="AA397" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB397" s="1">
+        <v>3</v>
+      </c>
+      <c r="AC397" s="1">
+        <v>54.7</v>
+      </c>
+      <c r="AM397" s="1" t="s">
+        <v>740</v>
+      </c>
+      <c r="AN397" s="1" t="s">
+        <v>740</v>
+      </c>
+      <c r="AO397" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP397" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AQ397" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AR397" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AS397" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AT397" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AW397" s="1" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="398" spans="3:50" x14ac:dyDescent="0.35">
+      <c r="C398" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="D398" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F398" s="1" t="s">
+        <v>1000</v>
+      </c>
+      <c r="G398" s="2">
+        <v>45188</v>
+      </c>
+      <c r="H398" s="50">
+        <v>0.30833333333333335</v>
+      </c>
+      <c r="L398" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M398" s="1" t="s">
+        <v>859</v>
+      </c>
+      <c r="N398" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="O398" s="1" t="s">
+        <v>666</v>
+      </c>
+      <c r="P398" s="1" t="s">
+        <v>1001</v>
+      </c>
+      <c r="Q398" s="3">
+        <v>3</v>
+      </c>
+      <c r="R398" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="S398" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="T398" s="4">
+        <v>20.7</v>
+      </c>
+      <c r="U398" s="1">
+        <v>2.4</v>
+      </c>
+      <c r="V398" s="1">
+        <v>690</v>
+      </c>
+      <c r="W398" s="1">
+        <v>637</v>
+      </c>
+      <c r="X398" s="1">
+        <v>7.45</v>
+      </c>
+      <c r="Y398" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="Z398" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="AA398" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB398" s="1">
+        <v>2</v>
+      </c>
+      <c r="AC398" s="1">
+        <v>24.5</v>
+      </c>
+      <c r="AM398" s="1" t="s">
+        <v>740</v>
+      </c>
+      <c r="AN398" s="1" t="s">
+        <v>740</v>
+      </c>
+      <c r="AO398" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP398" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AQ398" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AR398" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AS398" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AT398" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AW398" s="1" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="399" spans="3:50" x14ac:dyDescent="0.35">
+      <c r="C399" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="D399" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F399" s="1" t="s">
+        <v>1002</v>
+      </c>
+      <c r="G399" s="2">
+        <v>45188</v>
+      </c>
+      <c r="H399" s="50">
+        <v>0.38541666666666669</v>
+      </c>
+      <c r="L399" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M399" s="1" t="s">
+        <v>666</v>
+      </c>
+      <c r="N399" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="O399" s="1" t="s">
+        <v>859</v>
+      </c>
+      <c r="P399" s="1" t="s">
+        <v>1003</v>
+      </c>
+      <c r="Q399" s="3">
+        <v>3</v>
+      </c>
+      <c r="R399" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="S399" s="1">
+        <v>0.68</v>
+      </c>
+      <c r="T399" s="4">
+        <v>21.8</v>
+      </c>
+      <c r="U399" s="1">
+        <v>2.76</v>
+      </c>
+      <c r="V399" s="1">
+        <v>588</v>
+      </c>
+      <c r="W399" s="1">
+        <v>551</v>
+      </c>
+      <c r="X399" s="1">
+        <v>7.42</v>
+      </c>
+      <c r="Y399" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="Z399" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="AA399" s="1">
+        <v>1</v>
+      </c>
+      <c r="AC399" s="1">
+        <v>11</v>
+      </c>
+      <c r="AM399" s="1" t="s">
+        <v>740</v>
+      </c>
+      <c r="AN399" s="1" t="s">
+        <v>740</v>
+      </c>
+      <c r="AO399" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP399" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AQ399" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AR399" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AS399" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AT399" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AW399" s="1" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="400" spans="3:50" x14ac:dyDescent="0.35">
+      <c r="C400" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="D400" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F400" s="1" t="s">
+        <v>992</v>
+      </c>
+      <c r="G400" s="2">
+        <v>45188</v>
+      </c>
+      <c r="H400" s="50">
+        <v>0.47430555555555554</v>
+      </c>
+      <c r="L400" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M400" s="1" t="s">
+        <v>859</v>
+      </c>
+      <c r="N400" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="O400" s="1" t="s">
+        <v>987</v>
+      </c>
+      <c r="P400" s="1" t="s">
+        <v>993</v>
+      </c>
+      <c r="Q400" s="3">
+        <v>3</v>
+      </c>
+      <c r="R400" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="S400" s="1">
+        <v>0.32</v>
+      </c>
+      <c r="T400" s="4">
+        <v>21.6</v>
+      </c>
+      <c r="U400" s="1">
+        <v>7.79</v>
+      </c>
+      <c r="V400" s="1">
+        <v>412</v>
+      </c>
+      <c r="W400" s="1">
+        <v>385</v>
+      </c>
+      <c r="X400" s="1">
+        <v>7.94</v>
+      </c>
+      <c r="Y400" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="Z400" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="AA400" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB400" s="1">
+        <v>2</v>
+      </c>
+      <c r="AC400" s="1">
+        <v>19.100000000000001</v>
+      </c>
+      <c r="AD400" s="1">
+        <v>1815.3</v>
+      </c>
+      <c r="AE400" s="1">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AF400" s="1">
+        <v>0.27</v>
+      </c>
+      <c r="AG400" s="1">
+        <v>0.54</v>
+      </c>
+      <c r="AH400" s="1">
+        <v>1.85</v>
+      </c>
+      <c r="AI400" s="1">
+        <v>1356.1</v>
+      </c>
+      <c r="AJ400" s="1">
+        <v>908.5</v>
+      </c>
+      <c r="AK400" s="1">
+        <v>451.6</v>
+      </c>
+      <c r="AL400" s="1">
+        <v>18.5</v>
+      </c>
+      <c r="AM400" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AN400" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AO400" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP400" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AQ400" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AR400" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AS400" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AT400" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AW400" s="1" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="401" spans="3:49" x14ac:dyDescent="0.35">
+      <c r="C401" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="D401" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F401" s="1" t="s">
+        <v>1004</v>
+      </c>
+      <c r="G401" s="2">
+        <v>45188</v>
+      </c>
+      <c r="H401" s="50">
+        <v>0.39930555555555558</v>
+      </c>
+      <c r="L401" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M401" s="1" t="s">
+        <v>908</v>
+      </c>
+      <c r="N401" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="O401" s="1" t="s">
+        <v>887</v>
+      </c>
+      <c r="P401" s="1" t="s">
+        <v>1005</v>
+      </c>
+      <c r="Q401" s="3">
+        <v>2</v>
+      </c>
+      <c r="R401" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="S401" s="1">
+        <v>0.66</v>
+      </c>
+      <c r="T401" s="4">
+        <v>19.600000000000001</v>
+      </c>
+      <c r="U401" s="1">
+        <v>8.43</v>
+      </c>
+      <c r="V401" s="1">
+        <v>171</v>
+      </c>
+      <c r="W401" s="1">
+        <v>153</v>
+      </c>
+      <c r="X401" s="1">
+        <v>7.72</v>
+      </c>
+      <c r="Y401" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="Z401" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="AA401" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB401" s="1">
+        <v>2</v>
+      </c>
+      <c r="AC401" s="1">
+        <v>11.5</v>
+      </c>
+      <c r="AM401" s="1" t="s">
+        <v>740</v>
+      </c>
+      <c r="AN401" s="1" t="s">
+        <v>740</v>
+      </c>
+      <c r="AO401" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP401" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AQ401" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AR401" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AS401" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AT401" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AW401" s="1" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="402" spans="3:49" x14ac:dyDescent="0.35">
+      <c r="C402" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="D402" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="F402" s="1" t="s">
+        <v>1006</v>
+      </c>
+      <c r="G402" s="2">
+        <v>45188</v>
+      </c>
+      <c r="H402" s="50">
+        <v>0.375</v>
+      </c>
+      <c r="L402" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M402" s="1" t="s">
+        <v>908</v>
+      </c>
+      <c r="N402" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="O402" s="1" t="s">
+        <v>1007</v>
+      </c>
+      <c r="P402" s="1" t="s">
+        <v>1008</v>
+      </c>
+      <c r="Q402" s="3">
+        <v>2</v>
+      </c>
+      <c r="R402" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="S402" s="1">
+        <v>1.21</v>
+      </c>
+      <c r="T402" s="4">
+        <v>19.8</v>
+      </c>
+      <c r="U402" s="1">
+        <v>8.6199999999999992</v>
+      </c>
+      <c r="V402" s="1">
+        <v>166</v>
+      </c>
+      <c r="W402" s="1">
+        <v>150</v>
+      </c>
+      <c r="X402" s="1">
+        <v>7.72</v>
+      </c>
+      <c r="Y402" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="Z402" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="AA402" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB402" s="1">
+        <v>1</v>
+      </c>
+      <c r="AC402" s="1">
+        <v>6.4</v>
+      </c>
+      <c r="AM402" s="1" t="s">
+        <v>740</v>
+      </c>
+      <c r="AN402" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AO402" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP402" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AQ402" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AR402" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AS402" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AT402" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AW402" s="1" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="403" spans="3:49" x14ac:dyDescent="0.35">
+      <c r="C403" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="D403" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F403" s="1" t="s">
+        <v>1009</v>
+      </c>
+      <c r="G403" s="2">
+        <v>45188</v>
+      </c>
+      <c r="H403" s="50">
+        <v>0.35138888888888892</v>
+      </c>
+      <c r="L403" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M403" s="1" t="s">
+        <v>908</v>
+      </c>
+      <c r="N403" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="O403" s="1" t="s">
+        <v>1007</v>
+      </c>
+      <c r="P403" s="1" t="s">
+        <v>1008</v>
+      </c>
+      <c r="Q403" s="3">
+        <v>2</v>
+      </c>
+      <c r="R403" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="S403" s="1">
+        <v>1.36</v>
+      </c>
+      <c r="T403" s="4">
+        <v>20</v>
+      </c>
+      <c r="U403" s="1">
+        <v>8.6300000000000008</v>
+      </c>
+      <c r="V403" s="1">
+        <v>158</v>
+      </c>
+      <c r="W403" s="1">
+        <v>142</v>
+      </c>
+      <c r="X403" s="1">
+        <v>7.71</v>
+      </c>
+      <c r="Y403" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="Z403" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="AA403" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB403" s="1">
+        <v>1</v>
+      </c>
+      <c r="AC403" s="1">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="AM403" s="1" t="s">
+        <v>740</v>
+      </c>
+      <c r="AN403" s="1" t="s">
+        <v>740</v>
+      </c>
+      <c r="AO403" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP403" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AQ403" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AR403" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AS403" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AT403" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AW403" s="1" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="404" spans="3:49" x14ac:dyDescent="0.35">
+      <c r="C404" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="D404" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F404" s="1" t="s">
+        <v>1010</v>
+      </c>
+      <c r="G404" s="2">
+        <v>45188</v>
+      </c>
+      <c r="H404" s="50">
+        <v>0.32222222222222224</v>
+      </c>
+      <c r="L404" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M404" s="1" t="s">
+        <v>908</v>
+      </c>
+      <c r="N404" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="O404" s="1" t="s">
+        <v>887</v>
+      </c>
+      <c r="P404" s="1" t="s">
+        <v>1008</v>
+      </c>
+      <c r="Q404" s="3">
+        <v>2</v>
+      </c>
+      <c r="R404" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="S404" s="1">
+        <v>1.35</v>
+      </c>
+      <c r="T404" s="4">
+        <v>20</v>
+      </c>
+      <c r="U404" s="1">
+        <v>8.64</v>
+      </c>
+      <c r="V404" s="1">
+        <v>143</v>
+      </c>
+      <c r="W404" s="1">
+        <v>159</v>
+      </c>
+      <c r="X404" s="1">
+        <v>7.7</v>
+      </c>
+      <c r="Y404" s="1" t="s">
+        <v>905</v>
+      </c>
+      <c r="Z404" s="1" t="s">
+        <v>526</v>
+      </c>
+      <c r="AA404" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB404" s="1">
+        <v>1</v>
+      </c>
+      <c r="AC404" s="1">
+        <v>5</v>
+      </c>
+      <c r="AM404" s="1" t="s">
+        <v>740</v>
+      </c>
+      <c r="AN404" s="1" t="s">
+        <v>740</v>
+      </c>
+      <c r="AO404" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP404" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AQ404" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AR404" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AS404" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AT404" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AW404" s="1" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="405" spans="3:49" x14ac:dyDescent="0.35">
+      <c r="C405" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="D405" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="F405" s="1" t="s">
+        <v>1011</v>
+      </c>
+      <c r="G405" s="2">
+        <v>45188</v>
+      </c>
+      <c r="H405" s="50">
+        <v>0.28958333333333336</v>
+      </c>
+      <c r="L405" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M405" s="1" t="s">
+        <v>908</v>
+      </c>
+      <c r="N405" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="O405" s="1" t="s">
+        <v>1007</v>
+      </c>
+      <c r="P405" s="1" t="s">
+        <v>1008</v>
+      </c>
+      <c r="Q405" s="3">
+        <v>2</v>
+      </c>
+      <c r="R405" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="S405" s="1">
+        <v>1.35</v>
+      </c>
+      <c r="T405" s="4">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="U405" s="1">
+        <v>8.66</v>
+      </c>
+      <c r="V405" s="1">
+        <v>159</v>
+      </c>
+      <c r="W405" s="1">
+        <v>144.19999999999999</v>
+      </c>
+      <c r="X405" s="1">
+        <v>7.85</v>
+      </c>
+      <c r="Y405" s="1" t="s">
+        <v>905</v>
+      </c>
+      <c r="Z405" s="1" t="s">
+        <v>526</v>
+      </c>
+      <c r="AA405" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB405" s="1">
+        <v>1</v>
+      </c>
+      <c r="AC405" s="1">
+        <v>5.2</v>
+      </c>
+      <c r="AM405" s="1" t="s">
+        <v>740</v>
+      </c>
+      <c r="AN405" s="1" t="s">
+        <v>740</v>
+      </c>
+      <c r="AO405" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP405" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AQ405" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AR405" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AS405" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AT405" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AW405" s="1" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="406" spans="3:49" x14ac:dyDescent="0.35">
+      <c r="C406" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="D406" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F406" s="1" t="s">
+        <v>1012</v>
+      </c>
+      <c r="G406" s="2">
+        <v>45187</v>
+      </c>
+      <c r="H406" s="50">
+        <v>0.36388888888888887</v>
+      </c>
+      <c r="L406" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M406" s="1" t="s">
+        <v>843</v>
+      </c>
+      <c r="N406" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="O406" s="1" t="s">
+        <v>571</v>
+      </c>
+      <c r="P406" s="1" t="s">
+        <v>812</v>
+      </c>
+      <c r="Q406" s="3">
+        <v>2</v>
+      </c>
+      <c r="R406" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="S406" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="T406" s="4">
+        <v>19.5</v>
+      </c>
+      <c r="U406" s="1">
+        <v>8.7200000000000006</v>
+      </c>
+      <c r="V406" s="1">
+        <v>717</v>
+      </c>
+      <c r="W406" s="1">
+        <v>127</v>
+      </c>
+      <c r="X406" s="1">
+        <v>7.66</v>
+      </c>
+      <c r="Y406" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="Z406" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="AA406" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB406" s="1">
+        <v>1</v>
+      </c>
+      <c r="AC406" s="1">
+        <v>7</v>
+      </c>
+      <c r="AD406" s="1">
+        <v>1658.5</v>
+      </c>
+      <c r="AE406" s="1">
+        <v>0.06</v>
+      </c>
+      <c r="AF406" s="1">
+        <v>0.13</v>
+      </c>
+      <c r="AG406" s="1">
+        <v>0.74</v>
+      </c>
+      <c r="AH406" s="1">
+        <v>2.19</v>
+      </c>
+      <c r="AI406" s="1">
+        <v>1273.5</v>
+      </c>
+      <c r="AJ406" s="1">
+        <v>829.5</v>
+      </c>
+      <c r="AK406" s="1">
+        <v>414.3</v>
+      </c>
+      <c r="AL406" s="1">
+        <v>52.84</v>
+      </c>
+      <c r="AM406" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AN406" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AO406" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP406" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AQ406" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AR406" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AS406" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AT406" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AU406" s="1" t="s">
+        <v>1013</v>
+      </c>
+      <c r="AW406" s="1" t="s">
+        <v>582</v>
       </c>
     </row>
   </sheetData>
@@ -48453,15 +49943,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A42A54DAE8B40346B3F544786E5E866C" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b52beae5079fc7ce70e10e50a2e1ac64">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns3="cbc5ce0e-5942-45a9-8125-c067ee983ce7" xmlns:ns4="76d14374-bfe9-45d3-a0e1-d78b18a2be58" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="aa0f8a85f42a29e4236c61f71c44701a" ns1:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -48701,7 +50182,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
@@ -48710,15 +50191,16 @@
 </p:properties>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E9BC4319-F330-4E8C-9CD1-352735CB4D69}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F9AADF8-C019-4282-B74D-0079DF13966D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -48738,7 +50220,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD5C637B-81B8-44F6-B101-BBF6C0218B37}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="cbc5ce0e-5942-45a9-8125-c067ee983ce7"/>
@@ -48754,4 +50236,12 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E9BC4319-F330-4E8C-9CD1-352735CB4D69}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated with last transect data
</commit_message>
<xml_diff>
--- a/data/YBFMP_WQ_Data_WORKING_20221006.xlsx
+++ b/data/YBFMP_WQ_Data_WORKING_20221006.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eholmes\Documents\R\Projects\NDFS_reports\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70562BF3-B8F5-4ED4-A028-5FBE059AAAD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AD31FC0-8691-4567-8B25-A74ECECFC90C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" tabRatio="478" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="60" yWindow="-16310" windowWidth="29020" windowHeight="15820" tabRatio="478" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="3" r:id="rId1"/>
@@ -202,7 +202,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5420" uniqueCount="1018">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5622" uniqueCount="1047">
   <si>
     <t>Run Name</t>
   </si>
@@ -3515,6 +3515,93 @@
   </si>
   <si>
     <t>date changed from 9/6 to 9/7</t>
+  </si>
+  <si>
+    <t>changed secchi from 0.68 to 0.60</t>
+  </si>
+  <si>
+    <t>lots of algae in zoop samples</t>
+  </si>
+  <si>
+    <t>rounded EC to nearest whole number (150 to 151)</t>
+  </si>
+  <si>
+    <t>corrected secchi 1.36 to 1.35</t>
+  </si>
+  <si>
+    <t>2 RVB bottles missing, used extra bottled and added labels</t>
+  </si>
+  <si>
+    <t>corrected sp. Cond 717 to 141</t>
+  </si>
+  <si>
+    <t>ES1023B0600</t>
+  </si>
+  <si>
+    <t>moved 40m upstream.</t>
+  </si>
+  <si>
+    <t>ES1023B0601</t>
+  </si>
+  <si>
+    <t>aevans, eholmes</t>
+  </si>
+  <si>
+    <t>Lots of veg and shallow water</t>
+  </si>
+  <si>
+    <t>ES1023B0602</t>
+  </si>
+  <si>
+    <t>Turbid water in van dorn.</t>
+  </si>
+  <si>
+    <t>ES1023B0603</t>
+  </si>
+  <si>
+    <t>Barometric pressure 762.5</t>
+  </si>
+  <si>
+    <t>ES1023B0604</t>
+  </si>
+  <si>
+    <t>Collected Field Blank.</t>
+  </si>
+  <si>
+    <t>ES1023B0605</t>
+  </si>
+  <si>
+    <t>ES1023B0606</t>
+  </si>
+  <si>
+    <t>End of pole on light attenuation.</t>
+  </si>
+  <si>
+    <t>ES1023B0607</t>
+  </si>
+  <si>
+    <t>ES1023B0608</t>
+  </si>
+  <si>
+    <t>EL,AH,DD</t>
+  </si>
+  <si>
+    <t>ES1023B0609</t>
+  </si>
+  <si>
+    <t>ES1023B0610</t>
+  </si>
+  <si>
+    <t>ES1023B0611</t>
+  </si>
+  <si>
+    <t>Collected full process blank</t>
+  </si>
+  <si>
+    <t>ES1023B0612</t>
+  </si>
+  <si>
+    <t>lolson, nkwan</t>
   </si>
 </sst>
 </file>
@@ -3745,7 +3832,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3919,6 +4006,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="20" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4203,12 +4293,12 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:AX406"/>
+  <dimension ref="A1:AX419"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A397" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="AM1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A392" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="V403" sqref="V403"/>
+      <selection pane="bottomLeft" activeCell="AW419" sqref="AW419"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -47629,6 +47719,9 @@
       <c r="AW394" s="1" t="s">
         <v>582</v>
       </c>
+      <c r="AX394" s="1" t="s">
+        <v>987</v>
+      </c>
     </row>
     <row r="395" spans="3:50" x14ac:dyDescent="0.35">
       <c r="C395" s="1" t="s">
@@ -47932,6 +48025,9 @@
       <c r="AW397" s="1" t="s">
         <v>582</v>
       </c>
+      <c r="AX397" s="1" t="s">
+        <v>987</v>
+      </c>
     </row>
     <row r="398" spans="3:50" x14ac:dyDescent="0.35">
       <c r="C398" s="1" t="s">
@@ -48030,6 +48126,9 @@
       <c r="AW398" s="1" t="s">
         <v>582</v>
       </c>
+      <c r="AX398" s="1" t="s">
+        <v>987</v>
+      </c>
     </row>
     <row r="399" spans="3:50" x14ac:dyDescent="0.35">
       <c r="C399" s="1" t="s">
@@ -48069,7 +48168,7 @@
         <v>135</v>
       </c>
       <c r="S399" s="1">
-        <v>0.68</v>
+        <v>0.6</v>
       </c>
       <c r="T399" s="4">
         <v>21.8</v>
@@ -48122,8 +48221,14 @@
       <c r="AT399" s="1" t="b">
         <v>1</v>
       </c>
+      <c r="AV399" s="1" t="s">
+        <v>1018</v>
+      </c>
       <c r="AW399" s="1" t="s">
         <v>582</v>
+      </c>
+      <c r="AX399" s="1" t="s">
+        <v>987</v>
       </c>
     </row>
     <row r="400" spans="3:50" x14ac:dyDescent="0.35">
@@ -48250,8 +48355,11 @@
       <c r="AW400" s="1" t="s">
         <v>582</v>
       </c>
+      <c r="AX400" s="1" t="s">
+        <v>987</v>
+      </c>
     </row>
-    <row r="401" spans="3:49" x14ac:dyDescent="0.35">
+    <row r="401" spans="3:50" x14ac:dyDescent="0.35">
       <c r="C401" s="1" t="s">
         <v>255</v>
       </c>
@@ -48345,11 +48453,17 @@
       <c r="AT401" s="1" t="b">
         <v>1</v>
       </c>
+      <c r="AU401" s="1" t="s">
+        <v>1019</v>
+      </c>
       <c r="AW401" s="1" t="s">
         <v>582</v>
       </c>
+      <c r="AX401" s="1" t="s">
+        <v>987</v>
+      </c>
     </row>
-    <row r="402" spans="3:49" x14ac:dyDescent="0.35">
+    <row r="402" spans="3:50" x14ac:dyDescent="0.35">
       <c r="C402" s="1" t="s">
         <v>255</v>
       </c>
@@ -48399,7 +48513,7 @@
         <v>166</v>
       </c>
       <c r="W402" s="1">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="X402" s="1">
         <v>7.72</v>
@@ -48443,11 +48557,17 @@
       <c r="AT402" s="1" t="b">
         <v>1</v>
       </c>
+      <c r="AV402" s="1" t="s">
+        <v>1020</v>
+      </c>
       <c r="AW402" s="1" t="s">
         <v>582</v>
       </c>
+      <c r="AX402" s="1" t="s">
+        <v>987</v>
+      </c>
     </row>
-    <row r="403" spans="3:49" x14ac:dyDescent="0.35">
+    <row r="403" spans="3:50" x14ac:dyDescent="0.35">
       <c r="C403" s="1" t="s">
         <v>255</v>
       </c>
@@ -48485,7 +48605,7 @@
         <v>135</v>
       </c>
       <c r="S403" s="1">
-        <v>1.36</v>
+        <v>1.35</v>
       </c>
       <c r="T403" s="4">
         <v>20</v>
@@ -48541,11 +48661,17 @@
       <c r="AT403" s="1" t="b">
         <v>1</v>
       </c>
+      <c r="AV403" s="1" t="s">
+        <v>1021</v>
+      </c>
       <c r="AW403" s="1" t="s">
         <v>582</v>
       </c>
+      <c r="AX403" s="1" t="s">
+        <v>987</v>
+      </c>
     </row>
-    <row r="404" spans="3:49" x14ac:dyDescent="0.35">
+    <row r="404" spans="3:50" x14ac:dyDescent="0.35">
       <c r="C404" s="1" t="s">
         <v>255</v>
       </c>
@@ -48642,8 +48768,11 @@
       <c r="AW404" s="1" t="s">
         <v>582</v>
       </c>
+      <c r="AX404" s="1" t="s">
+        <v>987</v>
+      </c>
     </row>
-    <row r="405" spans="3:49" x14ac:dyDescent="0.35">
+    <row r="405" spans="3:50" x14ac:dyDescent="0.35">
       <c r="C405" s="1" t="s">
         <v>255</v>
       </c>
@@ -48737,11 +48866,17 @@
       <c r="AT405" s="1" t="b">
         <v>1</v>
       </c>
+      <c r="AU405" s="1" t="s">
+        <v>1022</v>
+      </c>
       <c r="AW405" s="1" t="s">
         <v>582</v>
       </c>
+      <c r="AX405" s="1" t="s">
+        <v>987</v>
+      </c>
     </row>
-    <row r="406" spans="3:49" x14ac:dyDescent="0.35">
+    <row r="406" spans="3:50" x14ac:dyDescent="0.35">
       <c r="C406" s="1" t="s">
         <v>383</v>
       </c>
@@ -48788,7 +48923,7 @@
         <v>8.7200000000000006</v>
       </c>
       <c r="V406" s="1">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="W406" s="1">
         <v>127</v>
@@ -48865,7 +49000,1360 @@
       <c r="AU406" s="1" t="s">
         <v>1013</v>
       </c>
+      <c r="AV406" s="1" t="s">
+        <v>1023</v>
+      </c>
       <c r="AW406" s="1" t="s">
+        <v>582</v>
+      </c>
+      <c r="AX406" s="1" t="s">
+        <v>987</v>
+      </c>
+    </row>
+    <row r="407" spans="3:50" x14ac:dyDescent="0.35">
+      <c r="C407" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="D407" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F407" s="1" t="s">
+        <v>1024</v>
+      </c>
+      <c r="G407" s="2">
+        <v>45202</v>
+      </c>
+      <c r="H407" s="50">
+        <v>0.39513888888888887</v>
+      </c>
+      <c r="L407" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M407" s="1" t="s">
+        <v>987</v>
+      </c>
+      <c r="N407" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="O407" s="1" t="s">
+        <v>847</v>
+      </c>
+      <c r="P407" s="1" t="s">
+        <v>971</v>
+      </c>
+      <c r="Q407" s="3">
+        <v>2</v>
+      </c>
+      <c r="R407" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="S407" s="1">
+        <v>0.26</v>
+      </c>
+      <c r="T407" s="4">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="U407" s="1">
+        <v>7.45</v>
+      </c>
+      <c r="V407" s="1">
+        <v>608</v>
+      </c>
+      <c r="W407" s="1">
+        <v>555</v>
+      </c>
+      <c r="X407" s="1">
+        <v>7.95</v>
+      </c>
+      <c r="Y407" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="Z407" s="1" t="s">
+        <v>526</v>
+      </c>
+      <c r="AA407" s="1">
+        <v>1</v>
+      </c>
+      <c r="AC407" s="1">
+        <v>21.7</v>
+      </c>
+      <c r="AM407" s="1" t="s">
+        <v>740</v>
+      </c>
+      <c r="AN407" s="1" t="s">
+        <v>740</v>
+      </c>
+      <c r="AO407" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP407" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AQ407" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AR407" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AS407" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AT407" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AU407" s="1" t="s">
+        <v>1025</v>
+      </c>
+      <c r="AW407" s="1" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="408" spans="3:50" x14ac:dyDescent="0.35">
+      <c r="C408" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="D408" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F408" s="1" t="s">
+        <v>1026</v>
+      </c>
+      <c r="G408" s="2">
+        <v>45202</v>
+      </c>
+      <c r="H408" s="50">
+        <v>0.34791666666666665</v>
+      </c>
+      <c r="L408" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M408" s="1" t="s">
+        <v>571</v>
+      </c>
+      <c r="N408" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="O408" s="1" t="s">
+        <v>987</v>
+      </c>
+      <c r="P408" s="1" t="s">
+        <v>1027</v>
+      </c>
+      <c r="Q408" s="3">
+        <v>2</v>
+      </c>
+      <c r="R408" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="S408" s="1">
+        <v>0.24</v>
+      </c>
+      <c r="T408" s="4">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="U408" s="1">
+        <v>4.43</v>
+      </c>
+      <c r="V408" s="1">
+        <v>789</v>
+      </c>
+      <c r="W408" s="1">
+        <v>720</v>
+      </c>
+      <c r="X408" s="1">
+        <v>7.18</v>
+      </c>
+      <c r="Y408" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="Z408" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="AA408" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB408" s="1">
+        <v>2</v>
+      </c>
+      <c r="AC408" s="1">
+        <v>25.1</v>
+      </c>
+      <c r="AM408" s="1" t="s">
+        <v>740</v>
+      </c>
+      <c r="AN408" s="1" t="s">
+        <v>740</v>
+      </c>
+      <c r="AO408" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP408" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AQ408" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AR408" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AS408" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AT408" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AU408" s="1" t="s">
+        <v>1028</v>
+      </c>
+      <c r="AW408" s="1" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="409" spans="3:50" x14ac:dyDescent="0.35">
+      <c r="C409" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="D409" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F409" s="1" t="s">
+        <v>1029</v>
+      </c>
+      <c r="G409" s="2">
+        <v>45202</v>
+      </c>
+      <c r="H409" s="50">
+        <v>0.28888888888888892</v>
+      </c>
+      <c r="L409" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M409" s="1" t="s">
+        <v>571</v>
+      </c>
+      <c r="N409" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="O409" s="1" t="s">
+        <v>987</v>
+      </c>
+      <c r="P409" s="1" t="s">
+        <v>1027</v>
+      </c>
+      <c r="Q409" s="3">
+        <v>2</v>
+      </c>
+      <c r="R409" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="S409" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="T409" s="4">
+        <v>18.2</v>
+      </c>
+      <c r="U409" s="1">
+        <v>2.59</v>
+      </c>
+      <c r="V409" s="1">
+        <v>542</v>
+      </c>
+      <c r="W409" s="1">
+        <v>472</v>
+      </c>
+      <c r="X409" s="1">
+        <v>7.26</v>
+      </c>
+      <c r="Y409" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="Z409" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="AA409" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB409" s="1">
+        <v>2</v>
+      </c>
+      <c r="AC409" s="1">
+        <v>15.3</v>
+      </c>
+      <c r="AM409" s="1" t="s">
+        <v>740</v>
+      </c>
+      <c r="AN409" s="1" t="s">
+        <v>740</v>
+      </c>
+      <c r="AO409" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP409" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AQ409" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AR409" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AS409" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AT409" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AU409" s="1" t="s">
+        <v>1030</v>
+      </c>
+      <c r="AW409" s="1" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="410" spans="3:50" x14ac:dyDescent="0.35">
+      <c r="C410" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="D410" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F410" s="1" t="s">
+        <v>1031</v>
+      </c>
+      <c r="G410" s="2">
+        <v>45202</v>
+      </c>
+      <c r="H410" s="50">
+        <v>0.47500000000000003</v>
+      </c>
+      <c r="L410" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M410" s="1" t="s">
+        <v>987</v>
+      </c>
+      <c r="N410" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="O410" s="1" t="s">
+        <v>571</v>
+      </c>
+      <c r="P410" s="1" t="s">
+        <v>918</v>
+      </c>
+      <c r="Q410" s="3">
+        <v>2</v>
+      </c>
+      <c r="R410" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="S410" s="1">
+        <v>0.23</v>
+      </c>
+      <c r="T410" s="4">
+        <v>18.5</v>
+      </c>
+      <c r="U410" s="1">
+        <v>6.49</v>
+      </c>
+      <c r="V410" s="1">
+        <v>538</v>
+      </c>
+      <c r="W410" s="1">
+        <v>471</v>
+      </c>
+      <c r="X410" s="1">
+        <v>7.64</v>
+      </c>
+      <c r="Y410" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="Z410" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="AA410" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB410" s="1">
+        <v>3</v>
+      </c>
+      <c r="AC410" s="1">
+        <v>26.9</v>
+      </c>
+      <c r="AM410" s="1" t="s">
+        <v>740</v>
+      </c>
+      <c r="AN410" s="1" t="s">
+        <v>740</v>
+      </c>
+      <c r="AO410" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP410" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AQ410" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AR410" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AS410" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AT410" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AU410" s="1" t="s">
+        <v>1032</v>
+      </c>
+      <c r="AW410" s="1" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="411" spans="3:50" x14ac:dyDescent="0.35">
+      <c r="C411" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="D411" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F411" s="1" t="s">
+        <v>1033</v>
+      </c>
+      <c r="G411" s="2">
+        <v>45202</v>
+      </c>
+      <c r="H411" s="50">
+        <v>0.31111111111111112</v>
+      </c>
+      <c r="L411" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M411" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="N411" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="O411" s="1" t="s">
+        <v>582</v>
+      </c>
+      <c r="P411" s="1" t="s">
+        <v>806</v>
+      </c>
+      <c r="Q411" s="3">
+        <v>1</v>
+      </c>
+      <c r="R411" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="S411" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="T411" s="4">
+        <v>17.7</v>
+      </c>
+      <c r="U411" s="1">
+        <v>4.42</v>
+      </c>
+      <c r="V411" s="1">
+        <v>669</v>
+      </c>
+      <c r="W411" s="1">
+        <v>576</v>
+      </c>
+      <c r="X411" s="1">
+        <v>7.44</v>
+      </c>
+      <c r="Y411" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="Z411" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="AA411" s="1">
+        <v>1</v>
+      </c>
+      <c r="AC411" s="1">
+        <v>22.5</v>
+      </c>
+      <c r="AM411" s="1" t="s">
+        <v>740</v>
+      </c>
+      <c r="AN411" s="1" t="s">
+        <v>740</v>
+      </c>
+      <c r="AO411" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP411" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AQ411" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AR411" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AS411" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AT411" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AU411" s="1" t="s">
+        <v>1034</v>
+      </c>
+      <c r="AW411" s="1" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="412" spans="3:50" x14ac:dyDescent="0.35">
+      <c r="C412" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="D412" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F412" s="1" t="s">
+        <v>1035</v>
+      </c>
+      <c r="G412" s="2">
+        <v>45202</v>
+      </c>
+      <c r="H412" s="50">
+        <v>0.37777777777777777</v>
+      </c>
+      <c r="L412" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M412" s="1" t="s">
+        <v>582</v>
+      </c>
+      <c r="N412" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="O412" s="1" t="s">
+        <v>666</v>
+      </c>
+      <c r="P412" s="1" t="s">
+        <v>793</v>
+      </c>
+      <c r="Q412" s="3">
+        <v>1</v>
+      </c>
+      <c r="R412" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="S412" s="1">
+        <v>0.24</v>
+      </c>
+      <c r="T412" s="4">
+        <v>20</v>
+      </c>
+      <c r="U412" s="1">
+        <v>6.94</v>
+      </c>
+      <c r="V412" s="1">
+        <v>696</v>
+      </c>
+      <c r="W412" s="1">
+        <v>628</v>
+      </c>
+      <c r="X412" s="1">
+        <v>7.93</v>
+      </c>
+      <c r="Y412" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="Z412" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="AA412" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB412" s="1">
+        <v>2</v>
+      </c>
+      <c r="AC412" s="1">
+        <v>32.6</v>
+      </c>
+      <c r="AM412" s="1" t="s">
+        <v>740</v>
+      </c>
+      <c r="AN412" s="1" t="s">
+        <v>740</v>
+      </c>
+      <c r="AO412" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP412" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AQ412" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AR412" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AS412" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AT412" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AW412" s="1" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="413" spans="3:50" x14ac:dyDescent="0.35">
+      <c r="C413" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="D413" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F413" s="1" t="s">
+        <v>1036</v>
+      </c>
+      <c r="G413" s="2">
+        <v>45202</v>
+      </c>
+      <c r="H413" s="50">
+        <v>0.4604166666666667</v>
+      </c>
+      <c r="L413" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M413" s="1" t="s">
+        <v>666</v>
+      </c>
+      <c r="N413" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="O413" s="1" t="s">
+        <v>582</v>
+      </c>
+      <c r="P413" s="1" t="s">
+        <v>925</v>
+      </c>
+      <c r="Q413" s="3">
+        <v>1</v>
+      </c>
+      <c r="R413" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="S413" s="1">
+        <v>0.45</v>
+      </c>
+      <c r="T413" s="4">
+        <v>19.5</v>
+      </c>
+      <c r="U413" s="1">
+        <v>8.36</v>
+      </c>
+      <c r="V413" s="1">
+        <v>200</v>
+      </c>
+      <c r="W413" s="1">
+        <v>178</v>
+      </c>
+      <c r="X413" s="1">
+        <v>7.96</v>
+      </c>
+      <c r="Y413" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="Z413" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="AA413" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB413" s="1">
+        <v>2</v>
+      </c>
+      <c r="AC413" s="1">
+        <v>12</v>
+      </c>
+      <c r="AD413" s="1">
+        <v>1736</v>
+      </c>
+      <c r="AE413" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="AF413" s="1">
+        <v>0.27</v>
+      </c>
+      <c r="AG413" s="1">
+        <v>0.71</v>
+      </c>
+      <c r="AH413" s="1">
+        <v>2.19</v>
+      </c>
+      <c r="AI413" s="1">
+        <v>1301.0999999999999</v>
+      </c>
+      <c r="AJ413" s="1">
+        <v>868.7</v>
+      </c>
+      <c r="AK413" s="1">
+        <v>424.6</v>
+      </c>
+      <c r="AL413" s="1">
+        <v>26.29</v>
+      </c>
+      <c r="AM413" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AN413" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AO413" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP413" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AQ413" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AR413" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AS413" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AT413" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AU413" s="1" t="s">
+        <v>1037</v>
+      </c>
+      <c r="AW413" s="1" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="414" spans="3:50" x14ac:dyDescent="0.35">
+      <c r="C414" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="D414" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F414" s="1" t="s">
+        <v>1038</v>
+      </c>
+      <c r="G414" s="2">
+        <v>45202</v>
+      </c>
+      <c r="H414" s="50">
+        <v>0.39027777777777778</v>
+      </c>
+      <c r="L414" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M414" s="1" t="s">
+        <v>603</v>
+      </c>
+      <c r="N414" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="O414" s="1" t="s">
+        <v>887</v>
+      </c>
+      <c r="P414" s="1" t="s">
+        <v>929</v>
+      </c>
+      <c r="Q414" s="3">
+        <v>3</v>
+      </c>
+      <c r="R414" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="S414" s="1">
+        <v>1.33</v>
+      </c>
+      <c r="T414" s="4">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="U414" s="1">
+        <v>8.84</v>
+      </c>
+      <c r="V414" s="1">
+        <v>145</v>
+      </c>
+      <c r="W414" s="1">
+        <v>127</v>
+      </c>
+      <c r="X414" s="1">
+        <v>7.68</v>
+      </c>
+      <c r="Y414" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="Z414" s="1" t="s">
+        <v>526</v>
+      </c>
+      <c r="AA414" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB414" s="1">
+        <v>2</v>
+      </c>
+      <c r="AC414" s="1">
+        <v>8.9</v>
+      </c>
+      <c r="AM414" s="1" t="s">
+        <v>740</v>
+      </c>
+      <c r="AN414" s="1" t="s">
+        <v>740</v>
+      </c>
+      <c r="AO414" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP414" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AQ414" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AR414" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AS414" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AT414" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AW414" s="1" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="415" spans="3:50" x14ac:dyDescent="0.35">
+      <c r="C415" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="D415" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="E415" s="61"/>
+      <c r="F415" s="1" t="s">
+        <v>1039</v>
+      </c>
+      <c r="G415" s="2">
+        <v>45202</v>
+      </c>
+      <c r="H415" s="50">
+        <v>0.37361111111111112</v>
+      </c>
+      <c r="L415" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M415" s="1" t="s">
+        <v>603</v>
+      </c>
+      <c r="N415" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="O415" s="1" t="s">
+        <v>908</v>
+      </c>
+      <c r="P415" s="1" t="s">
+        <v>1040</v>
+      </c>
+      <c r="Q415" s="3">
+        <v>3</v>
+      </c>
+      <c r="R415" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="S415" s="1">
+        <v>1.42</v>
+      </c>
+      <c r="T415" s="4">
+        <v>18.3</v>
+      </c>
+      <c r="U415" s="1">
+        <v>8.8800000000000008</v>
+      </c>
+      <c r="V415" s="1">
+        <v>132</v>
+      </c>
+      <c r="W415" s="1">
+        <v>115</v>
+      </c>
+      <c r="X415" s="1">
+        <v>7.55</v>
+      </c>
+      <c r="Y415" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="Z415" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="AA415" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB415" s="1">
+        <v>2</v>
+      </c>
+      <c r="AC415" s="1">
+        <v>7.9</v>
+      </c>
+      <c r="AM415" s="1" t="s">
+        <v>740</v>
+      </c>
+      <c r="AN415" s="1" t="s">
+        <v>740</v>
+      </c>
+      <c r="AO415" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP415" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AQ415" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AR415" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AS415" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AT415" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AW415" s="1" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="416" spans="3:50" x14ac:dyDescent="0.35">
+      <c r="C416" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="D416" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F416" s="1" t="s">
+        <v>1041</v>
+      </c>
+      <c r="G416" s="2">
+        <v>45202</v>
+      </c>
+      <c r="H416" s="50">
+        <v>0.35069444444444442</v>
+      </c>
+      <c r="L416" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M416" s="1" t="s">
+        <v>603</v>
+      </c>
+      <c r="N416" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="O416" s="1" t="s">
+        <v>908</v>
+      </c>
+      <c r="P416" s="1" t="s">
+        <v>1040</v>
+      </c>
+      <c r="Q416" s="3">
+        <v>3</v>
+      </c>
+      <c r="R416" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="S416" s="1">
+        <v>1.35</v>
+      </c>
+      <c r="T416" s="4">
+        <v>18.2</v>
+      </c>
+      <c r="U416" s="1">
+        <v>8.9</v>
+      </c>
+      <c r="V416" s="1">
+        <v>131</v>
+      </c>
+      <c r="W416" s="1">
+        <v>114</v>
+      </c>
+      <c r="X416" s="1">
+        <v>7.6</v>
+      </c>
+      <c r="Y416" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="Z416" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="AA416" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB416" s="1">
+        <v>1</v>
+      </c>
+      <c r="AC416" s="1">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="AM416" s="1" t="s">
+        <v>740</v>
+      </c>
+      <c r="AN416" s="1" t="s">
+        <v>740</v>
+      </c>
+      <c r="AO416" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP416" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AQ416" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AR416" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AS416" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AT416" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AW416" s="1" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="417" spans="3:49" x14ac:dyDescent="0.35">
+      <c r="C417" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="D417" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F417" s="1" t="s">
+        <v>1042</v>
+      </c>
+      <c r="G417" s="2">
+        <v>45202</v>
+      </c>
+      <c r="H417" s="50">
+        <v>0.32222222222222224</v>
+      </c>
+      <c r="L417" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M417" s="1" t="s">
+        <v>603</v>
+      </c>
+      <c r="N417" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="O417" s="1" t="s">
+        <v>908</v>
+      </c>
+      <c r="P417" s="1" t="s">
+        <v>1040</v>
+      </c>
+      <c r="Q417" s="3">
+        <v>3</v>
+      </c>
+      <c r="R417" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="S417" s="1">
+        <v>1.39</v>
+      </c>
+      <c r="T417" s="4">
+        <v>18.2</v>
+      </c>
+      <c r="U417" s="1">
+        <v>8.8699999999999992</v>
+      </c>
+      <c r="V417" s="1">
+        <v>131</v>
+      </c>
+      <c r="W417" s="1">
+        <v>114</v>
+      </c>
+      <c r="X417" s="1">
+        <v>7.59</v>
+      </c>
+      <c r="Y417" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="Z417" s="1" t="s">
+        <v>526</v>
+      </c>
+      <c r="AA417" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB417" s="1">
+        <v>1</v>
+      </c>
+      <c r="AC417" s="1">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="AM417" s="1" t="s">
+        <v>740</v>
+      </c>
+      <c r="AN417" s="1" t="s">
+        <v>740</v>
+      </c>
+      <c r="AO417" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP417" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AQ417" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AR417" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AS417" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AT417" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AW417" s="1" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="418" spans="3:49" x14ac:dyDescent="0.35">
+      <c r="C418" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="D418" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="F418" s="1" t="s">
+        <v>1043</v>
+      </c>
+      <c r="G418" s="2">
+        <v>45202</v>
+      </c>
+      <c r="H418" s="50">
+        <v>0.29305555555555557</v>
+      </c>
+      <c r="L418" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M418" s="1" t="s">
+        <v>603</v>
+      </c>
+      <c r="N418" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="O418" s="1" t="s">
+        <v>908</v>
+      </c>
+      <c r="P418" s="1" t="s">
+        <v>1040</v>
+      </c>
+      <c r="Q418" s="3">
+        <v>3</v>
+      </c>
+      <c r="R418" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="S418" s="1">
+        <v>1.49</v>
+      </c>
+      <c r="T418" s="4">
+        <v>18.3</v>
+      </c>
+      <c r="U418" s="1">
+        <v>8.81</v>
+      </c>
+      <c r="V418" s="1">
+        <v>130</v>
+      </c>
+      <c r="W418" s="1">
+        <v>114</v>
+      </c>
+      <c r="X418" s="1">
+        <v>7.54</v>
+      </c>
+      <c r="Y418" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="Z418" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="AA418" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB418" s="1">
+        <v>1</v>
+      </c>
+      <c r="AC418" s="1">
+        <v>7.2</v>
+      </c>
+      <c r="AM418" s="1" t="s">
+        <v>740</v>
+      </c>
+      <c r="AN418" s="1" t="s">
+        <v>740</v>
+      </c>
+      <c r="AO418" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP418" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AQ418" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AR418" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AS418" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AT418" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AU418" s="1" t="s">
+        <v>1044</v>
+      </c>
+      <c r="AW418" s="1" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="419" spans="3:49" x14ac:dyDescent="0.35">
+      <c r="C419" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="D419" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F419" s="1" t="s">
+        <v>1045</v>
+      </c>
+      <c r="G419" s="2">
+        <v>45202</v>
+      </c>
+      <c r="H419" s="50">
+        <v>0.39444444444444443</v>
+      </c>
+      <c r="L419" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M419" s="1" t="s">
+        <v>571</v>
+      </c>
+      <c r="N419" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="O419" s="1" t="s">
+        <v>582</v>
+      </c>
+      <c r="P419" s="1" t="s">
+        <v>1046</v>
+      </c>
+      <c r="Q419" s="3">
+        <v>1</v>
+      </c>
+      <c r="R419" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="S419" s="1">
+        <v>1.76</v>
+      </c>
+      <c r="T419" s="4">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="U419" s="1">
+        <v>9.17</v>
+      </c>
+      <c r="V419" s="1">
+        <v>111</v>
+      </c>
+      <c r="W419" s="1">
+        <v>95</v>
+      </c>
+      <c r="X419" s="1">
+        <v>7.38</v>
+      </c>
+      <c r="Y419" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="Z419" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="AA419" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB419" s="1">
+        <v>1</v>
+      </c>
+      <c r="AC419" s="1">
+        <v>6.6</v>
+      </c>
+      <c r="AD419" s="1">
+        <v>1789.9</v>
+      </c>
+      <c r="AE419" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="AF419" s="1">
+        <v>0.18</v>
+      </c>
+      <c r="AG419" s="1">
+        <v>0.91</v>
+      </c>
+      <c r="AH419" s="1">
+        <v>2.19</v>
+      </c>
+      <c r="AI419" s="1">
+        <v>1343.1</v>
+      </c>
+      <c r="AJ419" s="1">
+        <v>896.6</v>
+      </c>
+      <c r="AK419" s="1">
+        <v>449.5</v>
+      </c>
+      <c r="AL419" s="1">
+        <v>174.1</v>
+      </c>
+      <c r="AM419" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AN419" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AO419" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP419" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AQ419" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AR419" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AS419" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AT419" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AU419" s="1" t="s">
+        <v>1037</v>
+      </c>
+      <c r="AW419" s="1" t="s">
         <v>582</v>
       </c>
     </row>
@@ -49943,6 +51431,24 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A42A54DAE8B40346B3F544786E5E866C" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b52beae5079fc7ce70e10e50a2e1ac64">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns3="cbc5ce0e-5942-45a9-8125-c067ee983ce7" xmlns:ns4="76d14374-bfe9-45d3-a0e1-d78b18a2be58" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="aa0f8a85f42a29e4236c61f71c44701a" ns1:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -50182,25 +51688,33 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD5C637B-81B8-44F6-B101-BBF6C0218B37}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="cbc5ce0e-5942-45a9-8125-c067ee983ce7"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="76d14374-bfe9-45d3-a0e1-d78b18a2be58"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E9BC4319-F330-4E8C-9CD1-352735CB4D69}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F9AADF8-C019-4282-B74D-0079DF13966D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -50218,30 +51732,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E9BC4319-F330-4E8C-9CD1-352735CB4D69}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD5C637B-81B8-44F6-B101-BBF6C0218B37}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="cbc5ce0e-5942-45a9-8125-c067ee983ce7"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="76d14374-bfe9-45d3-a0e1-d78b18a2be58"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>